<commit_message>
finished match summary export
</commit_message>
<xml_diff>
--- a/CSharpZapoctak/Resources/match_summary.xlsx
+++ b/CSharpZapoctak/Resources/match_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riki1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68843EDD-B626-4DED-8E6A-EC1FCC1CF0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAF0F02-EC04-4786-9532-833B6C6C767B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,12 +74,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -178,82 +186,85 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="45" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="45" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="45" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="45" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -822,7 +833,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33:K33"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,8 +850,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
       <c r="C1" s="3"/>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -858,17 +869,17 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -879,683 +890,607 @@
     </row>
     <row r="8" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="H8" s="27" t="s">
+      <c r="D8" s="16"/>
+      <c r="H8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="27"/>
+      <c r="I8" s="16"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E11" s="26"/>
-      <c r="F11" s="26" t="s">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="26"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="20"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-      <c r="K49" s="20"/>
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="21"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="22"/>
-      <c r="K52" s="22"/>
+      <c r="A52" s="23"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="24"/>
+      <c r="J52" s="24"/>
+      <c r="K52" s="24"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="17"/>
-      <c r="K53" s="17"/>
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K55" s="28"/>
+      <c r="K55" s="13"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D58" s="13"/>
+      <c r="D58" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="92">
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:J10"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="G21:K21"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="G29:K29"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="G31:K31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="G36:K36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="G37:K37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="G38:K38"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="G39:K39"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="G40:K40"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="G41:K41"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="G42:K42"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="G43:K43"/>
-    <mergeCell ref="G49:K49"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="G44:K44"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="G45:K45"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="G46:K46"/>
     <mergeCell ref="A53:E53"/>
     <mergeCell ref="G53:K53"/>
     <mergeCell ref="B54:E54"/>
@@ -1572,6 +1507,82 @@
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="G48:K48"/>
     <mergeCell ref="A49:E49"/>
+    <mergeCell ref="G49:K49"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="G44:K44"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="G45:K45"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="G41:K41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="G42:K42"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="G43:K43"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="G38:K38"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="G39:K39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="G40:K40"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="G36:K36"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="G37:K37"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="G29:K29"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="G31:K31"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:J10"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.2" bottom="0.3" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>